<commit_message>
Adjusted code and examples to new requirements
</commit_message>
<xml_diff>
--- a/employee-list.xlsx
+++ b/employee-list.xlsx
@@ -145,12 +145,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7975708502024"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -178,7 +178,6 @@
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -188,7 +187,6 @@
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>

</xml_diff>